<commit_message>
dma added, compare event is used, compare value is updated on update event (preload enabled)
</commit_message>
<xml_diff>
--- a/doc/calc.xlsx
+++ b/doc/calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\work\2023\neopixel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA00221-4230-405F-8763-E2E713130C08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B56D04C-0831-48E8-9990-DB0069C084C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54542C48-6B14-413D-AA62-40A53A46CE07}"/>
+    <workbookView xWindow="5490" yWindow="1830" windowWidth="18255" windowHeight="13020" xr2:uid="{54542C48-6B14-413D-AA62-40A53A46CE07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Timer calculator</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>ms</t>
+  </si>
+  <si>
+    <t>-&gt;</t>
+  </si>
+  <si>
+    <t>1.25 us per</t>
+  </si>
+  <si>
+    <t>.4us pos width</t>
   </si>
 </sst>
 </file>
@@ -253,7 +262,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -270,6 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -340,13 +350,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>513575</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>114987</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -724,15 +734,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28288CCF-D52E-40A4-966D-03562BFA0ADC}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -891,7 +902,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="9">
-        <v>65535</v>
+        <v>119</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>11</v>
@@ -925,7 +936,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="9">
-        <v>200</v>
+        <v>76</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>11</v>
@@ -959,15 +970,15 @@
         <v>12</v>
       </c>
       <c r="D14" s="10">
-        <f>D5/(D8+1)/D10</f>
-        <v>1.4648661020828565E-3</v>
+        <f>D5/(D8+1)/(D10+1)</f>
+        <v>0.8</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="10">
         <f>1/D14</f>
-        <v>682.65625</v>
+        <v>1.25</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>17</v>
@@ -984,14 +995,14 @@
       <c r="C15" s="7"/>
       <c r="D15" s="10">
         <f>D14*1000</f>
-        <v>1.4648661020828564</v>
+        <v>800</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="10">
         <f>1/D15</f>
-        <v>0.68265625000000008</v>
+        <v>1.25E-3</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>18</v>
@@ -1008,7 +1019,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="11">
         <f>D15*1000</f>
-        <v>1464.8661020828563</v>
+        <v>800000</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>16</v>
@@ -1029,41 +1040,51 @@
       </c>
       <c r="D17" s="10">
         <f>D12/D10*100</f>
-        <v>0.30518043793392846</v>
+        <v>63.865546218487388</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
+      <c r="F17" s="10">
+        <f>F14*D17/100</f>
+        <v>0.79831932773109227</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="10">
+        <f>F17*1000</f>
+        <v>798.31932773109224</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1101,9 +1122,15 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="C22" s="1">
+        <v>119</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1115,9 +1142,13 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1">
+        <v>38</v>
+      </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1129,9 +1160,13 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1">
+        <v>76</v>
+      </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1">
+        <v>0.79800000000000004</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1303,6 +1338,10 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
@@ -1314,6 +1353,16 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>